<commit_message>
defines added, demo program
</commit_message>
<xml_diff>
--- a/Pomiar czasu/kosztorys.xlsx
+++ b/Pomiar czasu/kosztorys.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="8505"/>
+    <workbookView xWindow="10740" yWindow="-120" windowWidth="9750" windowHeight="8850"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="62">
   <si>
     <t>transceiver RFM69HW-433S2</t>
   </si>
@@ -175,13 +175,40 @@
   </si>
   <si>
     <t>RC0805JR-071KL</t>
+  </si>
+  <si>
+    <t>Stabilizator 5V, 0,5A</t>
+  </si>
+  <si>
+    <t>LF50CDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stabilizato 3,3V, </t>
+  </si>
+  <si>
+    <t>LF33 - 3.3V/1A</t>
+  </si>
+  <si>
+    <t>DIP Switch 4-biegowy czerwony</t>
+  </si>
+  <si>
+    <t>Gniazdo zasilające DC 2.1/5.5</t>
+  </si>
+  <si>
+    <t>RC0805JR-0739RL</t>
+  </si>
+  <si>
+    <t>rezystor 39R</t>
+  </si>
+  <si>
+    <t>Cewka 10uH 1.2A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,12 +216,6 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF404040"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -247,7 +268,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -425,11 +446,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -479,16 +511,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -498,7 +521,21 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -800,25 +837,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -841,7 +887,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -858,18 +904,18 @@
         <v>12.44</v>
       </c>
       <c r="F3" s="8">
-        <f>D3*E3</f>
+        <f t="shared" ref="F3:F30" si="0">D3*E3</f>
         <v>74.64</v>
       </c>
       <c r="G3" s="12">
-        <f>ROUND(1.23*F3,2)</f>
+        <f t="shared" ref="G3:G21" si="1">ROUND(1.23*F3,2)</f>
         <v>91.81</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -886,16 +932,16 @@
         <v>4.16</v>
       </c>
       <c r="F4" s="8">
-        <f t="shared" ref="F4:F24" si="0">D4*E4</f>
+        <f t="shared" si="0"/>
         <v>49.92</v>
       </c>
       <c r="G4" s="12">
-        <f>ROUND(1.23*F4,2)</f>
+        <f t="shared" si="1"/>
         <v>61.4</v>
       </c>
-      <c r="H4" s="21"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -912,16 +958,16 @@
         <v>0.99</v>
       </c>
       <c r="F5" s="8">
-        <f t="shared" ref="F5" si="1">D5*E5</f>
+        <f t="shared" si="0"/>
         <v>11.879999999999999</v>
       </c>
       <c r="G5" s="12">
-        <f>ROUND(1.23*F5,2)</f>
+        <f t="shared" si="1"/>
         <v>14.61</v>
       </c>
-      <c r="H5" s="21"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H5" s="24"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -932,22 +978,22 @@
         <v>16</v>
       </c>
       <c r="D6" s="6">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E6" s="13">
         <v>0.21</v>
       </c>
       <c r="F6" s="8">
         <f t="shared" si="0"/>
-        <v>2.52</v>
+        <v>3.78</v>
       </c>
       <c r="G6" s="12">
-        <f>ROUND(1.23*F6,2)</f>
-        <v>3.1</v>
-      </c>
-      <c r="H6" s="21"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -968,12 +1014,12 @@
         <v>3.4139999999999997</v>
       </c>
       <c r="G7" s="12">
-        <f t="shared" ref="G7:G21" si="2">ROUND(1.23*F7,2)</f>
+        <f t="shared" si="1"/>
         <v>4.2</v>
       </c>
-      <c r="H7" s="21"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H7" s="24"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -994,12 +1040,12 @@
         <v>20.04</v>
       </c>
       <c r="G8" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>24.65</v>
       </c>
-      <c r="H8" s="21"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H8" s="24"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -1020,12 +1066,12 @@
         <v>2.5</v>
       </c>
       <c r="G9" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.08</v>
       </c>
-      <c r="H9" s="21"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H9" s="24"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -1046,12 +1092,12 @@
         <v>4.8540000000000001</v>
       </c>
       <c r="G10" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.97</v>
       </c>
-      <c r="H10" s="21"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H10" s="24"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -1072,38 +1118,38 @@
         <v>3.2460000000000004</v>
       </c>
       <c r="G11" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.99</v>
       </c>
-      <c r="H11" s="21"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H11" s="24"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="D12" s="6">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E12" s="13">
-        <v>0.8</v>
+        <v>1.98</v>
       </c>
       <c r="F12" s="8">
         <f t="shared" si="0"/>
-        <v>9.6000000000000014</v>
+        <v>11.879999999999999</v>
       </c>
       <c r="G12" s="12">
-        <f t="shared" si="2"/>
-        <v>11.81</v>
-      </c>
-      <c r="H12" s="21"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>14.61</v>
+      </c>
+      <c r="H12" s="24"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -1124,12 +1170,12 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.08</v>
       </c>
-      <c r="H13" s="21"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H13" s="24"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -1150,13 +1196,12 @@
         <v>3.2</v>
       </c>
       <c r="G14" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.94</v>
       </c>
-      <c r="H14" s="21"/>
-      <c r="L14" s="26"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -1177,12 +1222,12 @@
         <v>3.2</v>
       </c>
       <c r="G15" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.94</v>
       </c>
-      <c r="H15" s="21"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H15" s="24"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -1203,10 +1248,10 @@
         <v>4.7054999999999998</v>
       </c>
       <c r="G16" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.79</v>
       </c>
-      <c r="H16" s="21"/>
+      <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
@@ -1229,36 +1274,36 @@
         <v>2.1</v>
       </c>
       <c r="G17" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.58</v>
       </c>
-      <c r="H17" s="21"/>
+      <c r="H17" s="24"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="D18" s="6">
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="E18" s="13">
-        <v>0.59</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F18" s="8">
         <f t="shared" si="0"/>
-        <v>3.54</v>
+        <v>2.5</v>
       </c>
       <c r="G18" s="12">
-        <f t="shared" si="2"/>
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="H18" s="21"/>
+        <f t="shared" si="1"/>
+        <v>3.08</v>
+      </c>
+      <c r="H18" s="24"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
@@ -1281,10 +1326,10 @@
         <v>3.2600000000000002</v>
       </c>
       <c r="G19" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.01</v>
       </c>
-      <c r="H19" s="14"/>
+      <c r="H19" s="19"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
@@ -1307,10 +1352,10 @@
         <v>4.3600000000000003</v>
       </c>
       <c r="G20" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.36</v>
       </c>
-      <c r="H20" s="14"/>
+      <c r="H20" s="19"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
@@ -1329,14 +1374,14 @@
         <v>0.20862</v>
       </c>
       <c r="F21" s="8">
-        <f>D21*E21</f>
+        <f t="shared" si="0"/>
         <v>4.1723999999999997</v>
       </c>
       <c r="G21" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.13</v>
       </c>
-      <c r="H21" s="14"/>
+      <c r="H21" s="19"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
@@ -1360,7 +1405,7 @@
         <f>F22</f>
         <v>22.200000000000003</v>
       </c>
-      <c r="H22" s="22" t="s">
+      <c r="H22" s="25" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1383,10 +1428,10 @@
         <v>19.899999999999999</v>
       </c>
       <c r="G23" s="11">
-        <f t="shared" ref="G23:G26" si="3">F23</f>
+        <f t="shared" ref="G23:G24" si="2">F23</f>
         <v>19.899999999999999</v>
       </c>
-      <c r="H23" s="22"/>
+      <c r="H23" s="25"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
@@ -1407,86 +1452,184 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="G24" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.9499999999999993</v>
       </c>
-      <c r="H24" s="22"/>
+      <c r="H24" s="25"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>23</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="15"/>
+        <v>55</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>56</v>
+      </c>
       <c r="D25" s="15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E25" s="16">
-        <v>1.4</v>
+        <v>2.11</v>
       </c>
       <c r="F25" s="17">
-        <f>D25*E25</f>
-        <v>7</v>
-      </c>
-      <c r="G25" s="18">
+        <f t="shared" si="0"/>
+        <v>12.66</v>
+      </c>
+      <c r="G25" s="17">
         <f>F25</f>
-        <v>7</v>
-      </c>
-      <c r="H25" s="22"/>
-    </row>
-    <row r="26" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12.66</v>
+      </c>
+      <c r="H25" s="25"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>24</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15">
+        <v>6</v>
+      </c>
+      <c r="E26" s="16">
+        <v>0.59</v>
+      </c>
+      <c r="F26" s="17">
+        <f t="shared" si="0"/>
+        <v>3.54</v>
+      </c>
+      <c r="G26" s="23">
+        <f>F26</f>
+        <v>3.54</v>
+      </c>
+      <c r="H26" s="25"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>25</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15">
+        <v>18</v>
+      </c>
+      <c r="E27" s="16">
+        <v>0.44</v>
+      </c>
+      <c r="F27" s="17">
+        <f t="shared" si="0"/>
+        <v>7.92</v>
+      </c>
+      <c r="G27" s="23">
+        <f>F27</f>
+        <v>7.92</v>
+      </c>
+      <c r="H27" s="25"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>26</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15">
+        <v>10</v>
+      </c>
+      <c r="E28" s="16">
+        <v>0.25</v>
+      </c>
+      <c r="F28" s="17">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G28" s="23">
+        <f>F28</f>
+        <v>2.5</v>
+      </c>
+      <c r="H28" s="25"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>27</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15">
+        <v>5</v>
+      </c>
+      <c r="E29" s="16">
+        <v>1.4</v>
+      </c>
+      <c r="F29" s="17">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G29" s="18">
+        <f>F29</f>
+        <v>7</v>
+      </c>
+      <c r="H29" s="25"/>
+    </row>
+    <row r="30" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>28</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6">
+      <c r="C30" s="6"/>
+      <c r="D30" s="6">
         <v>5</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E30" s="13">
         <v>30.62</v>
       </c>
-      <c r="F26" s="23">
-        <f>D26*E26</f>
+      <c r="F30" s="20">
+        <f t="shared" si="0"/>
         <v>153.1</v>
       </c>
-      <c r="G26" s="24">
-        <f>F26</f>
+      <c r="G30" s="21">
+        <f>F30</f>
         <v>153.1</v>
       </c>
-      <c r="H26" s="25" t="s">
+      <c r="H30" s="22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="19" t="s">
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="10">
-        <f>SUM(F3:F26)</f>
-        <v>425.80190000000005</v>
-      </c>
-      <c r="G27" s="7">
-        <f>SUM(G3:G26)</f>
-        <v>474.94999999999993</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D30" s="1"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="10">
+        <f>SUM(F3:F30)</f>
+        <v>454.92190000000005</v>
+      </c>
+      <c r="G31" s="7">
+        <f>SUM(G3:G30)</f>
+        <v>504.65000000000009</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A27:E27"/>
     <mergeCell ref="H3:H18"/>
-    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="H22:H29"/>
+    <mergeCell ref="A31:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1495,12 +1638,710 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="6">
+        <v>6</v>
+      </c>
+      <c r="E2" s="13">
+        <v>12.44</v>
+      </c>
+      <c r="F2" s="8">
+        <f t="shared" ref="F2:F23" si="0">D2*E2</f>
+        <v>74.64</v>
+      </c>
+      <c r="G2" s="12">
+        <f t="shared" ref="G2:G20" si="1">ROUND(1.23*F2,2)</f>
+        <v>91.81</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6">
+        <v>12</v>
+      </c>
+      <c r="E3" s="13">
+        <v>4.16</v>
+      </c>
+      <c r="F3" s="8">
+        <f t="shared" si="0"/>
+        <v>49.92</v>
+      </c>
+      <c r="G3" s="12">
+        <f t="shared" si="1"/>
+        <v>61.4</v>
+      </c>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="6">
+        <v>12</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0.99</v>
+      </c>
+      <c r="F4" s="8">
+        <f t="shared" si="0"/>
+        <v>11.879999999999999</v>
+      </c>
+      <c r="G4" s="12">
+        <f t="shared" si="1"/>
+        <v>14.61</v>
+      </c>
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="6">
+        <v>12</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0.21</v>
+      </c>
+      <c r="F5" s="8">
+        <f t="shared" si="0"/>
+        <v>2.52</v>
+      </c>
+      <c r="G5" s="12">
+        <f t="shared" si="1"/>
+        <v>3.1</v>
+      </c>
+      <c r="H5" s="24"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="6">
+        <v>6</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="F6" s="8">
+        <f t="shared" si="0"/>
+        <v>3.4139999999999997</v>
+      </c>
+      <c r="G6" s="12">
+        <f t="shared" si="1"/>
+        <v>4.2</v>
+      </c>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="6">
+        <v>6</v>
+      </c>
+      <c r="E7" s="13">
+        <v>3.34</v>
+      </c>
+      <c r="F7" s="8">
+        <f t="shared" si="0"/>
+        <v>20.04</v>
+      </c>
+      <c r="G7" s="12">
+        <f t="shared" si="1"/>
+        <v>24.65</v>
+      </c>
+      <c r="H7" s="24"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="6">
+        <v>100</v>
+      </c>
+      <c r="E8" s="13">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G8" s="12">
+        <f t="shared" si="1"/>
+        <v>3.08</v>
+      </c>
+      <c r="H8" s="24"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="6">
+        <v>6</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="F9" s="8">
+        <f t="shared" si="0"/>
+        <v>4.8540000000000001</v>
+      </c>
+      <c r="G9" s="12">
+        <f t="shared" si="1"/>
+        <v>5.97</v>
+      </c>
+      <c r="H9" s="24"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="6">
+        <v>6</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="F10" s="8">
+        <f t="shared" si="0"/>
+        <v>3.2460000000000004</v>
+      </c>
+      <c r="G10" s="12">
+        <f t="shared" si="1"/>
+        <v>3.99</v>
+      </c>
+      <c r="H10" s="24"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="6">
+        <v>12</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="F11" s="8">
+        <f t="shared" si="0"/>
+        <v>9.6000000000000014</v>
+      </c>
+      <c r="G11" s="12">
+        <f t="shared" si="1"/>
+        <v>11.81</v>
+      </c>
+      <c r="H11" s="24"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="6">
+        <v>100</v>
+      </c>
+      <c r="E12" s="13">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F12" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G12" s="12">
+        <f t="shared" si="1"/>
+        <v>3.08</v>
+      </c>
+      <c r="H12" s="24"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="6">
+        <v>100</v>
+      </c>
+      <c r="E13" s="13">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="F13" s="8">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+      <c r="G13" s="12">
+        <f t="shared" si="1"/>
+        <v>3.94</v>
+      </c>
+      <c r="H13" s="24"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="6">
+        <v>100</v>
+      </c>
+      <c r="E14" s="13">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="F14" s="8">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+      <c r="G14" s="12">
+        <f t="shared" si="1"/>
+        <v>3.94</v>
+      </c>
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="6">
+        <v>50</v>
+      </c>
+      <c r="E15" s="13">
+        <v>9.4109999999999999E-2</v>
+      </c>
+      <c r="F15" s="8">
+        <f t="shared" si="0"/>
+        <v>4.7054999999999998</v>
+      </c>
+      <c r="G15" s="12">
+        <f t="shared" si="1"/>
+        <v>5.79</v>
+      </c>
+      <c r="H15" s="24"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="6">
+        <v>25</v>
+      </c>
+      <c r="E16" s="13">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="F16" s="8">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+      <c r="G16" s="12">
+        <f t="shared" si="1"/>
+        <v>2.58</v>
+      </c>
+      <c r="H16" s="24"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="6">
+        <v>25</v>
+      </c>
+      <c r="E17" s="13">
+        <v>0.59</v>
+      </c>
+      <c r="F17" s="8">
+        <f t="shared" si="0"/>
+        <v>14.75</v>
+      </c>
+      <c r="G17" s="12">
+        <f t="shared" si="1"/>
+        <v>18.14</v>
+      </c>
+      <c r="H17" s="24"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="6">
+        <v>20</v>
+      </c>
+      <c r="E18" s="13">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="F18" s="8">
+        <f t="shared" si="0"/>
+        <v>3.2600000000000002</v>
+      </c>
+      <c r="G18" s="12">
+        <f t="shared" si="1"/>
+        <v>4.01</v>
+      </c>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="6">
+        <v>20</v>
+      </c>
+      <c r="E19" s="13">
+        <v>0.218</v>
+      </c>
+      <c r="F19" s="8">
+        <f t="shared" si="0"/>
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="G19" s="12">
+        <f t="shared" si="1"/>
+        <v>5.36</v>
+      </c>
+      <c r="H19" s="14"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="6">
+        <v>20</v>
+      </c>
+      <c r="E20" s="13">
+        <v>0.20862</v>
+      </c>
+      <c r="F20" s="8">
+        <f t="shared" si="0"/>
+        <v>4.1723999999999997</v>
+      </c>
+      <c r="G20" s="12">
+        <f t="shared" si="1"/>
+        <v>5.13</v>
+      </c>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6">
+        <v>7</v>
+      </c>
+      <c r="E21" s="13">
+        <v>3.7</v>
+      </c>
+      <c r="F21" s="9">
+        <f t="shared" si="0"/>
+        <v>25.900000000000002</v>
+      </c>
+      <c r="G21" s="11">
+        <f>F21</f>
+        <v>25.900000000000002</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6">
+        <v>10</v>
+      </c>
+      <c r="E22" s="13">
+        <v>1.99</v>
+      </c>
+      <c r="F22" s="9">
+        <f t="shared" si="0"/>
+        <v>19.899999999999999</v>
+      </c>
+      <c r="G22" s="11">
+        <f>F22</f>
+        <v>19.899999999999999</v>
+      </c>
+      <c r="H22" s="25"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6">
+        <v>5</v>
+      </c>
+      <c r="E23" s="13">
+        <v>1.99</v>
+      </c>
+      <c r="F23" s="9">
+        <f t="shared" si="0"/>
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="G23" s="11">
+        <f>F23</f>
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="H23" s="25"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="25"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="25"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="25"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>23</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15">
+        <v>5</v>
+      </c>
+      <c r="E27" s="16">
+        <v>1.4</v>
+      </c>
+      <c r="F27" s="17">
+        <f>D27*E27</f>
+        <v>7</v>
+      </c>
+      <c r="G27" s="18">
+        <f>F27</f>
+        <v>7</v>
+      </c>
+      <c r="H27" s="25"/>
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>24</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6">
+        <v>5</v>
+      </c>
+      <c r="E28" s="13">
+        <v>30.62</v>
+      </c>
+      <c r="F28" s="20">
+        <f>D28*E28</f>
+        <v>153.1</v>
+      </c>
+      <c r="G28" s="21">
+        <f>F28</f>
+        <v>153.1</v>
+      </c>
+      <c r="H28" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="10">
+        <f>SUM(F2:F28)</f>
+        <v>440.71190000000001</v>
+      </c>
+      <c r="G29" s="7">
+        <f>SUM(G2:G28)</f>
+        <v>492.43999999999994</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="H2:H17"/>
+    <mergeCell ref="H21:H27"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>